<commit_message>
Updated files with new changes
</commit_message>
<xml_diff>
--- a/literature review.xlsx
+++ b/literature review.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Bachelor\Literature Review\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Bachelor\Literature Review\Literature Review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E15F7252-D42A-411A-B89C-5CDB384942B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3436373D-15FE-452D-A0FF-0E5FD1095091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{1D23A328-8199-4E04-8381-B399FD7168CE}"/>
   </bookViews>
@@ -40,7 +40,7 @@
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="7">
+  <futureMetadata name="XLRICHVALUE" count="8">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -90,8 +90,15 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="7"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
-  <valueMetadata count="7">
+  <valueMetadata count="8">
     <bk>
       <rc t="1" v="0"/>
     </bk>
@@ -113,12 +120,15 @@
     <bk>
       <rc t="1" v="6"/>
     </bk>
+    <bk>
+      <rc t="1" v="7"/>
+    </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="431">
   <si>
     <t>index</t>
   </si>
@@ -204,51 +214,10 @@
     <t>Luong Vuong Nguyen</t>
   </si>
   <si>
-    <t xml:space="preserve">2024
-</t>
-  </si>
-  <si>
     <t>Journal</t>
   </si>
   <si>
-    <t>1-The paper identifies challenges in implementing Swarm Intelligence (SI) in multi-robotic systems, such as scalability, robustness, communication, coordination, heterogeneity, energy efficiency, adaptability, and security.
-2-It highlights the unpredictability of swarm systems due to the complexity of interactions among robots, which can lead to undesired emergent behaviors.
-3-The paper also points out the limited individual capabilities of swarm robots, which restrict the types of tasks they can perform and the environments in which they can operate effectively.</t>
-  </si>
-  <si>
-    <t>1-To provide a comprehensive review of Swarm Intelligence (SI) and its application to multi-robot systems.
-2-To explore the foundational principles, algorithms, and practical implementations of SI in multi-robotics.
-3-To identify the key challenges and limitations of using SI in multi-robot systems and propose future research directions.</t>
-  </si>
-  <si>
-    <t>used but names not mentioned</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-1-Mathematical Benchmarking Functions:
--Rastrigin function and Schwefel function to simulate the search and rescue environment.
--Randomized Constrained Optimization Functions: Additional randomized constrained optimization functions were used to generate random contours and mimic real-world search scenarios.
-2-IoT Devices</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-1-To provide an overview of the foundational principles and algorithms of Swarm Intelligence.
-2-To examine the application of SI in key domains such as search and rescue, environmental monitoring, agriculture, and space exploration.
-3-To identify and discuss the primary challenges and risks of using SI in multi-robot systems.
-4-To propose future research directions for improving the reliability and effectiveness of SI in multi-robotics.</t>
-  </si>
-  <si>
     <t>Sensors Used</t>
-  </si>
-  <si>
-    <t>Convergence Speed: How quickly the algorithm finds an optimal solution.
-Scalability: How well the algorithm performs as the number of robots or problem size increases.
-Robustness: The ability to handle individual robot failures without degrading performance.
-Energy Efficiency: Minimizing energy consumption while performing tasks.
-Adaptability: Adjusting to dynamic environments and unexpected changes.
-Communication and Coordination: Ensuring reliable information exchange and coordination among robots.
-Task Efficiency: Completing tasks efficiently, such as covering an area or avoiding obstacles.
-Data Reliability: Ensuring the accuracy and reliability of data collected by the swarm.</t>
   </si>
   <si>
     <t>Marc-André Blais, Moulay A. Akhloufi</t>
@@ -492,17 +461,6 @@
   </si>
   <si>
     <t>Department of Artificial Intelligence, FPT University, Danang, Vietnam</t>
-  </si>
-  <si>
-    <t>MDPI, Basel, Switzerland</t>
-  </si>
-  <si>
-    <t>Swarm intelligence
-Multi-robotics
-Swarm robots</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Swarm Intelligence</t>
   </si>
   <si>
     <t>Lewis M. Pyke and Craig R. Stark</t>
@@ -1489,14 +1447,6 @@
 The paper reviews existing methods and highlights the need for a robust collision avoidance algorithm that can be integrated with PSO without affecting its search efficiency, making UAV-based SAR missions more practical and effective.</t>
   </si>
   <si>
-    <t>Swarm Intelligence (SI) is inspired by natural systems like ants, bees, and birds, focusing on decentralized, self-organized, and emergent behaviors.
-SI algorithms (e.g., ACO, PSO, FA, CS, BA) are widely used for optimization, path planning, and task allocation in multi-robot systems.
-Applications include search and rescue, environmental monitoring, agriculture, and space exploration, where SI enhances scalability, robustness, and adaptability.
-Challenges involve scalability, communication, coordination, energy efficiency, and real-world implementation in dynamic environments.
-Limitations include unpredictable emergent behaviors, reliance on local information, and hardware constraints.
-Future research aims to improve individual robot capabilities, develop robust algorithms, and integrate AI for better decision-making in swarm systems.</t>
-  </si>
-  <si>
     <t>Swarm robotics leverages decentralized control of multiple robots, inspired by natural systems like ants and birds, to solve complex tasks.
 Reinforcement Learning (RL) is increasingly used to enable autonomous decision-making in swarm systems, improving efficiency and adaptability.
 Applications include forest fire prevention, agriculture, logistics, military operations, and search and rescue missions, where swarms of drones and ground robots perform tasks like monitoring, target tracking, and disaster response.
@@ -1507,15 +1457,6 @@
     <t>Model</t>
   </si>
   <si>
-    <t>Applied Math</t>
-  </si>
-  <si>
-    <t>1-The paper provides a detailed taxonomy of The paper provides a detailed taxonomy of Swarm Intelligence research, categorizing significant contributions and areas of focus within the field.
-2-It offers a comprehensive review of SI algorithms and their applications in multi-robotics.
-3-The paper identifies key challenges and limitations of SI in multi-robot systems and suggests future research directions to address these issues.
-4-It highlights the versatility and potential impact of SI across various sectors, including search and rescue, environmental monitoring, agriculture, and space exploration. Swarm Intelligence research, categorizing significant contributions and areas of focus within the field.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> optimization methods; multi-criteria methods for decision making (MCDM); analysis
  and decision making; metaheuristics; particle swarm algorithm (PSO)</t>
   </si>
@@ -1544,6 +1485,562 @@
 Memory Efficiency: Memory allocation per frame.
 Pathfinding Accuracy: Time taken to complete the objective (find the target), number of collisions (drone-to-environment and drone-to-drone).
 Initialization Time: Time required to set up the simulation.</t>
+  </si>
+  <si>
+    <t>Maria-Theresa Oanh Hoang, Kasper Andreas Rømer Grøntved, Niels van Berkel, Mikael B. Skov, Anders Lyhne Christensen, and Timothy Merritt</t>
+  </si>
+  <si>
+    <t>Aalborg University, Aalborg, Denmark (Hoang, van Berkel, Skov, Merritt)
+University of Southern Denmark, Odense, Denmark (Grøntved, Christensen)</t>
+  </si>
+  <si>
+    <t>Springer Nature Switzerland AG</t>
+  </si>
+  <si>
+    <t>Cultural Robotics: Social Robots and Their Emergent Cultural Ecologies</t>
+  </si>
+  <si>
+    <t>Drone swarms, search and rescue (SAR), human-swarm interaction, situational awareness, visualization, team culture, public perception, emergency services, UAVs, swarm behavior, swarm control interfaces.</t>
+  </si>
+  <si>
+    <t>search and rescue , Drone swarms.</t>
+  </si>
+  <si>
+    <t>Limited understanding of how drone swarms can be integrated into the working practices of emergency response teams.
+Lack of research on user interfaces for controlling and managing drone swarms in SAR operations.
+Insufficient exploration of the interaction between drone swarms and other parties in the airspace.
+Public perception and acceptance of drone swarms in SAR missions remain underexplored.</t>
+  </si>
+  <si>
+    <t>Develop more advanced swarm control interfaces that balance simplicity and functionality.
+Conduct further studies on the feasibility of monitoring multiple drone feeds simultaneously.
+Investigate the role of automation in reducing operator workload and improving situational awareness.
+Explore public perception and ways to communicate the purpose of drone swarms during SAR missions.
+Test and evaluate the effectiveness of drone swarms in various SAR scenarios, including residential areas.</t>
+  </si>
+  <si>
+    <t>To explore the challenges and opportunities of using drone swarms in search and rescue operations, focusing on the development of user interfaces for swarm control and the integration of drone swarms into emergency response practices.</t>
+  </si>
+  <si>
+    <t>UAVs for Emergency Settings: UAVs are increasingly used in emergency situations due to their short deployment time and ability to minimize human involvement in hazardous environments. They are used for visual surveillance, firefighting, and SAR missions.
+UAV Swarm Behavior and Control: Research has explored algorithms for autonomous swarm behavior, inspired by animal swarms (e.g., bees, birds). Control methods include leader-follower models, beacon controls, and automated search patterns.
+User Interfaces for Human-Swarm Interaction: Controlling multiple drones simultaneously requires interfaces that reduce visual clutter and maintain situational awareness. Studies emphasize the importance of displaying only key information to avoid overwhelming the operator.</t>
+  </si>
+  <si>
+    <t>To investigate the challenges and opportunities of using drone swarms in SAR operations, focusing on user interface design, situational awareness, and integration into emergency response practices.</t>
+  </si>
+  <si>
+    <t>Identified five key research challenges for drone swarms in SAR: visualization, situational awareness, technical issues, team culture, and public perception.
+Developed initial prototypes for drone swarm control interfaces and conducted evaluations with emergency services personnel.
+Provided insights into the potential benefits and challenges of transitioning from single drones to drone swarms in SAR missions.</t>
+  </si>
+  <si>
+    <t>Interviews with emergency services personnel (Danish Emergency Management Agency - DEMA).
+Prototype development for drone swarm control interfaces using web technologies and DJI flight controllers.
+Physical drones for demonstration and evaluation.</t>
+  </si>
+  <si>
+    <t>Visualization: The prototype interface was evaluated for its ability to provide clear and concise information to operators.
+Situational Awareness: The study explored how operators could maintain awareness of multiple drones and their feeds.
+Technical Issues: The robustness of the system in harsh conditions and the need for backup devices were discussed.
+Team Culture: The impact of drone swarms on team dynamics and roles was considered.
+Public Perception: The potential public reaction to drone swarms in SAR missions was explored.</t>
+  </si>
+  <si>
+    <t>Cameras (visible light and thermal imaging).
+Microphones.
+Loudspeakers.</t>
+  </si>
+  <si>
+    <t>Constraints</t>
+  </si>
+  <si>
+    <t>Tests or Tasks</t>
+  </si>
+  <si>
+    <t>Attributes</t>
+  </si>
+  <si>
+    <t>Drone Battery: Limited flight time due to battery capacity.
+Terrain and Weather: Harsh conditions can affect drone performance.
+Communication: Ensuring reliable communication between multiple drones and the operator.
+Public Perception: Managing how the public perceives drone swarms during SAR missions.
+Regulatory Compliance: Adhering to flight regulations, especially in residential areas.</t>
+  </si>
+  <si>
+    <t>Search Patterns: Testing different search patterns (e.g., spiral, scatter) for drone swarms.
+Situational Awareness: Evaluating how operators manage multiple drone feeds.
+Automation: Testing the effectiveness of automated detection and alert systems.
+Public Interaction: Exploring ways to communicate with the public during SAR missions.
+Team Dynamics: Assessing how the introduction of drone swarms affects team roles and responsibilities.</t>
+  </si>
+  <si>
+    <t>AppliedMath</t>
+  </si>
+  <si>
+    <t>Swarm intelligence, multi-robotics, swarm robots, decentralized systems, self-organization, emergent behavior, Ant Colony Optimization (ACO), Particle Swarm Optimization (PSO), Firefly Algorithm (FA), Cuckoo Search (CS), Bat Algorithm (BA).</t>
+  </si>
+  <si>
+    <t>Swarm intelligence, swarm robots, decentralized systems, self-organization, emergent behavior, Particle Swarm Optimization (PSO).</t>
+  </si>
+  <si>
+    <t>Limited understanding of how swarm intelligence (SI) can be effectively applied to multi-robot systems in real-world scenarios.
+Challenges in scalability, robustness, communication, and coordination in large-scale swarm robotics.
+Lack of comprehensive frameworks for integrating heterogeneous robots with varying capabilities into cohesive swarm systems.
+Insufficient exploration of the unpredictability of emergent behaviors in swarm systems.
+Need for more research on energy efficiency and adaptability in dynamic environments.</t>
+  </si>
+  <si>
+    <t>Develop more advanced swarm control algorithms that balance local autonomy with global coordination.
+Investigate the integration of AI and machine learning to enhance decision-making in swarm robotics.
+Explore hybrid approaches that combine local and global information sharing to improve swarm performance.
+Conduct extensive field testing to bridge the gap between theoretical models and real-world applications.
+Focus on reducing maintenance and scalability costs through modular design and advanced manufacturing techniques.
+Address security concerns in swarm robotics, particularly in sensitive or hostile environments.</t>
+  </si>
+  <si>
+    <t>To provide a comprehensive review of swarm intelligence (SI) and its application to multi-robot systems, highlighting foundational principles, key algorithms, practical implementations, challenges, and future directions.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foundational Concepts: SI is inspired by the collective behavior of social insects like ants, bees, and birds. Key principles include decentralization, self-organization, emergent behavior, and local interactions.
+SI Algorithms: The paper reviews various SI algorithms, including Ant Colony Optimization (ACO), Particle Swarm Optimization (PSO), Firefly Algorithm (FA), Cuckoo Search (CS), and Bat Algorithm (BA). These algorithms are inspired by natural behaviors and have been applied to optimization problems in multi-robot systems.
+Applications: SI has been applied in search and rescue, environmental monitoring, agriculture, and space exploration. These applications leverage the robustness, scalability, and adaptability of swarm systems.
+Challenges: Key challenges include scalability, robustness, communication, coordination, heterogeneity, energy efficiency, adaptability, and security.
+Limitations: Limitations of SI-based multi-robotics include limited individual robot capabilities, algorithmic complexity, unpredictability, dependence on local information, interference, and difficulty in real-world implementation.
+</t>
+  </si>
+  <si>
+    <t>To provide an overview of the foundational principles and algorithms of swarm intelligence.
+To examine the application of SI in key domains such as search and rescue, environmental monitoring, agriculture, and space exploration.
+To identify and discuss the primary challenges and risks of using SI in multi-robot systems.
+To propose future research directions and strategies for improving the reliability and effectiveness of SI in multi-robotics.</t>
+  </si>
+  <si>
+    <t>Provides a detailed taxonomy of swarm intelligence research, categorizing key contributions and areas of focus.
+Explores a wide range of applications where SI can be effectively deployed, demonstrating its versatility and potential impact.
+Identifies and analyzes the primary challenges of implementing SI in multi-robotic systems, offering insights into current limitations and areas requiring further research.
+Discusses the inherent limitations of SI and suggests possible solutions to overcome these barriers.</t>
+  </si>
+  <si>
+    <t>Literature review of peer-reviewed journal articles, conference papers, and book chapters from reputable sources (IEEE, Springer, ACM, etc.).
+Analysis of SI algorithms (ACO, PSO, FA, CS, BA) and their applications in multi-robot systems.
+Case studies and examples of swarm robotics in various domains.</t>
+  </si>
+  <si>
+    <t>Convergence Speed: How quickly the algorithm approaches an optimal solution.
+Scalability: The ability to maintain performance as the number of robots increases.
+Complexity: Computational demands and ease of implementation.
+Suitability for Dynamic Environments: The ability to adapt to changes in the environment or problem parameters.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> reviews various swarm intelligence algorithms (ACO, PSO, FA, CS, BA) and their applications in multi-robot systems.</t>
+  </si>
+  <si>
+    <t>Cameras (for environmental monitoring and search and rescue).
+Thermal sensors (for detecting heat signatures in search and rescue).
+Air quality sensors (for environmental monitoring).
+Humidity and temperature sensors (for environmental monitoring).
+Echolocation sensors (inspired by the Bat Algorithm).</t>
+  </si>
+  <si>
+    <t>Scalability: Maintaining efficiency as the number of robots increases.
+Robustness: Handling individual robot failures without degrading overall performance.
+Communication: Ensuring reliable information exchange among robots in dynamic environments.
+Energy Efficiency: Minimizing energy consumption for extended operation in remote or harsh environments.
+Adaptability: Adjusting to changes in terrain, obstacles, and environmental conditions.
+Security: Protecting the swarm from malicious attacks or rogue robots.</t>
+  </si>
+  <si>
+    <t>Search and Rescue: Robots must navigate complex environments to locate and assist distressed individuals.
+Environmental Monitoring: Robots must cover large areas to collect data on air quality, temperature, humidity, and vegetation health.
+Agriculture: Robots must perform tasks such as planting, pest control, and harvesting in large agricultural fields.
+Space Exploration: Robots must map planetary surfaces, discover resources, and construct habitats in harsh environments.</t>
+  </si>
+  <si>
+    <t>Zool Hilmi Ismail, Mohd Ghazali Mohd Hamami</t>
+  </si>
+  <si>
+    <t>Centre for Artificial Intelligence and Robotics, Universiti Teknologi Malaysia, Kuala Lumpur, Malaysia
+Malaysia-Japan International Institute of Technology, Universiti Teknologi Malaysia, Kuala Lumpur, Malaysia
+Faculty of Mechanical Engineering, Universiti Teknologi MARA Cawangan Johor, Malaysia</t>
+  </si>
+  <si>
+    <t>Applied Sciences (Appl. Sci.)</t>
+  </si>
+  <si>
+    <t>Artificial Intelligence , Swarm Intelligence , Swarm Robotics , Systematic Literature Review , Target Search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Artificial Intelligence , Swarm Intelligence , Swarm Robotics </t>
+  </si>
+  <si>
+    <t>Most studies focus on static environments, with limited exploration of dynamic environments.
+Few papers validate their algorithms on real robot platforms, relying mostly on simulations.
+Lack of mathematical models for swarm robot interactions and convergence proofs.
+Limited exploration of hybrid strategies combining multiple techniques.</t>
+  </si>
+  <si>
+    <t>Dynamic Environment Testing: Future research should test SR strategies in dynamic environments with various target types and values.
+Real Robot Platform Validation: More experiments should be conducted on real robot platforms to bridge the gap between simulation and real-world applications.
+Mathematical Modeling: Derive mathematical models of swarm robot interactions and design controllers with convergence proofs.
+Hybrid Strategies: Explore hybrid strategies that combine multiple techniques to overcome individual limitations.</t>
+  </si>
+  <si>
+    <t>To provide a systematic literature review (SLR) of swarm robotics (SR) strategies applied to target search problems with environmental constraints, highlighting current state-of-the-art approaches, their performance, and future research directions.</t>
+  </si>
+  <si>
+    <t>The paper reviews 25 selected articles from 2009 to 2020, focusing on SR strategies for target search problems. The strategies are categorized into four main mechanisms:
+Bio-inspired Mechanisms: Inspired by natural behaviors like flocking, foraging, and stigmergy.
+Behavior-based Mechanisms: Focus on subsumption architecture and sensor-based behaviors.
+Random Strategy Mechanisms: Use random walk methods like Brownian motion and Lévy flight.
+Hybrid Mechanisms: Combine multiple strategies to enhance performance.
+The review highlights the dominance of Particle Swarm Optimization (PSO) in SR strategies due to its simplicity and effectiveness in global optimization problems. However, PSO has limitations, such as getting trapped in local minima. Behavior-based strategies are flexible but computationally intensive, while random walk strategies are simple but lose effectiveness as swarm size increases.</t>
+  </si>
+  <si>
+    <t>To systematically review and analyze SR strategies applied to target search problems, identify research gaps, and provide future recommendations.</t>
+  </si>
+  <si>
+    <t>A comprehensive review of SR strategies for target search problems.
+Identification of key research gaps and future directions.
+Classification of strategies into bio-inspired, behavior-based, random, and hybrid mechanisms.
+Highlighting the dominance of PSO and its limitations.</t>
+  </si>
+  <si>
+    <t>Algorithms: Particle Swarm Optimization (PSO), Behavior-based strategies, Random Walk (Brownian motion, Lévy flight), Hybrid strategies.</t>
+  </si>
+  <si>
+    <t>Virtual Robot Experimental Platform (V-REP): Used for simulation-based validation.
+Kilobots Robot Platform: Used for real robot validation in some studies.</t>
+  </si>
+  <si>
+    <t>Success Rate: Percentage of successful target searches.
+Energy Consumption: Efficiency in energy usage during search tasks.
+Time Consumption: Time taken to locate targets.
+Adaptability: Ability to adapt to dynamic environments.
+Scalability: Performance with varying swarm sizes.</t>
+  </si>
+  <si>
+    <t>Local Sensing: Robots are equipped with local sensing capabilities for obstacle avoidance and target detection.
+RFID Tags: Used in some studies for stigmergy-based communication.
+Vision and Pressure Sensors: Used in behavior-based strategies for input data.</t>
+  </si>
+  <si>
+    <t>Environment Complexity: Empty space vs. cluttered environments.
+Target Mobility: Static vs. dynamic targets.
+Swarm Size: Scalability issues with large swarms.
+Energy Constraints: Limited battery life for robots.
+Time Constraints: Survivors may have limited time, requiring fast search algorithms.</t>
+  </si>
+  <si>
+    <t>Target Search: Locate single or multiple targets in a given environment.
+Obstacle Avoidance: Navigate around obstacles in cluttered environments.
+Energy Efficiency: Optimize energy consumption during search tasks.
+Scalability Testing: Evaluate performance with varying swarm sizes.
+Dynamic Environment Testing: Test algorithms in environments with moving targets or changing conditions.</t>
+  </si>
+  <si>
+    <t>Dariusz Marek, Marcin Paszkuta, Jakub Szygula, Piotr Biernacki, Adam Domanski, Marta Szczygieł, Marcel Król, Konrad Wojciechowski</t>
+  </si>
+  <si>
+    <t>Department of Distributed Systems and Informatic Devices, Faculty of Automatic Control, Electronics and Computer Science, Silesian University of Technology, Poland
+Polish-Japanese Academy of Information Technology, Poland
+Polish Academy of Sciences, Institute of Theoretical and Applied Informatics, Poland</t>
+  </si>
+  <si>
+    <t>Swarm of drones , Swarm robotics , Software-in-the-loop (SITL) , Industry 4.0 , Simulation environments , Collision avoidance , Positioning accuracy , Communication delays</t>
+  </si>
+  <si>
+    <t>Swarm of drones , Swarm robotics , Collision avoidance , Positioning accuracy , Communication delays</t>
+  </si>
+  <si>
+    <t>Limited exploration of dynamic environments in drone swarm simulations.
+Lack of real-world validation for swarm control algorithms.
+Need for advanced collision avoidance mechanisms in high-speed swarm operations.
+Insufficient focus on the impact of communication delays and positioning errors on swarm coordination.</t>
+  </si>
+  <si>
+    <t>Dynamic Environment Testing: Future research should test swarm control algorithms in dynamic environments with moving obstacles and targets.
+Real-World Validation: Conduct experiments with real drones to validate simulation results and bridge the gap between simulation and real-world applications.
+Advanced Collision Avoidance: Develop more sophisticated collision avoidance mechanisms to enable high-speed swarm operations.
+Improved Communication Systems: Enhance communication systems to reduce delays and improve swarm coordination in complex environments.</t>
+  </si>
+  <si>
+    <t>To explore the role of software-in-the-loop (SITL) simulations in developing, testing, and validating drone swarm control algorithms, focusing on operational efficiency, adaptability, and collision avoidance in various scenarios.</t>
+  </si>
+  <si>
+    <t>The paper reviews the growing importance of drone swarms in various domains, including environmental monitoring, crisis management, and military applications. It discusses the challenges of controlling drone swarms, such as communication delays, positioning errors, and collision avoidance. The authors highlight the use of simulation methods, particularly SITL, for testing and validating swarm control algorithms. The paper also references foundational works on swarm robotics, distributed consensus models, and the application of swarm intelligence in adaptive routing and formation control.</t>
+  </si>
+  <si>
+    <t>To analyze the impact of positioning errors, communication delays, and swarm speed on the coordination and collision avoidance capabilities of drone swarms in a simulated environment.</t>
+  </si>
+  <si>
+    <t>A detailed analysis of the impact of GPS positioning errors and communication delays on swarm coordination.
+Development of a leader-based control mechanism for drone swarms.
+Simulation-based validation of swarm control algorithms using SITL.
+Identification of minimum safe distances between drones to avoid collisions under various conditions.</t>
+  </si>
+  <si>
+    <t>Algorithms: Leader-based control mechanism, collision avoidance algorithms.
+                                                                                                                                                                                                                                           Hardware: Holybro X500 frame, Pixhawk 6C flight controller, Raspberry Pi 4B, RTK GPS modules.
+Software: ArduPilot flight management software, custom Python-based swarm control software.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microsoft AirSim: Used for SITL simulations to test and validate swarm control algorithms.
+</t>
+  </si>
+  <si>
+    <t>Minimum Distance Between Drones: The minimum safe distance required to avoid collisions under different conditions.
+Swarm Speed: The maximum safe speed at which the swarm can operate without collisions.
+Positioning Accuracy: The impact of GPS positioning errors on swarm coordination.
+Communication Delays: The effect of communication delays on swarm synchronization and collision avoidance.</t>
+  </si>
+  <si>
+    <t>Leader-Based Control Model: The swarm follows a leader drone, with each drone mimicking the leader's trajectory and movements. This model ensures coherent coordination and collision avoidance within the swarm.</t>
+  </si>
+  <si>
+    <t>GPS RTK Modules: For precise positioning and navigation.
+WiFi Communication Modules: For real-time communication between drones and the ground control station.
+Sensors for Environmental Interaction: Not explicitly mentioned, but drones are equipped with sensors for obstacle detection and collision avoidance.</t>
+  </si>
+  <si>
+    <t>Positioning Errors: GPS inaccuracies can affect swarm coordination and collision avoidance.
+Communication Delays: Delays in data transmission can lead to synchronization issues and collisions.
+Swarm Speed: Higher speeds increase the risk of collisions, especially in dense formations.
+Battery Life: Limited battery capacity restricts the operational time of drones.
+Environmental Complexity: Obstacles and dynamic environments can challenge swarm coordination.</t>
+  </si>
+  <si>
+    <t>Formation Maintenance: Drones must maintain a specific formation (e.g., grid structure) while navigating.
+Collision Avoidance: Drones must avoid collisions with each other and obstacles.
+Speed Variation: Drones must operate at varying speeds (1–5 m/s) while maintaining formation.
+Communication Testing: The impact of communication delays (0 ms to 500 ms) on swarm coordination is tested.
+Positioning Accuracy: The effect of GPS positioning errors (0 cm, 5 cm, 50 cm, 100 cm) on swarm coordination is evaluated.</t>
+  </si>
+  <si>
+    <t>Abhishek Phadke, F. Antonio Medrano, Chandra N. Sekharan, Tianxing Chu</t>
+  </si>
+  <si>
+    <t>Conrad Blucher Institute for Surveying and Science, Texas A&amp;M University-Corpus Christi, USA
+Department of Computer Science, Texas A&amp;M University-Corpus Christi, USA</t>
+  </si>
+  <si>
+    <t>MDPI</t>
+  </si>
+  <si>
+    <t>Sensors</t>
+  </si>
+  <si>
+    <t>UAV , Swarm , Robotics , Simulation , Experiment design , Swarm resilience , Search and rescue , Heterogeneous agents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Swarm , Robotics  , Search and rescue </t>
+  </si>
+  <si>
+    <t>Lack of standardized experimental procedures for validating UAV swarm systems.
+Limited exploration of dynamic environments in swarm simulations.
+Insufficient focus on the interoperability of simulation platforms for complex swarm experiments.
+Need for comprehensive testing of swarm resilience and performance in diverse scenarios.</t>
+  </si>
+  <si>
+    <t>Dynamic Environment Testing: Future research should test swarm control algorithms in dynamic environments with moving obstacles and targets.
+Real-World Validation: Conduct experiments with real drones to validate simulation results and bridge the gap between simulation and real-world applications.
+Advanced Collision Avoidance: Develop more sophisticated collision avoidance mechanisms to enable high-speed swarm operations.
+Improved Communication Systems: Enhance communication systems to reduce delays and improve swarm coordination in complex environments.
+Interoperability of Simulation Platforms: Explore the integration of multiple simulation platforms to handle complex multimodal experiments.</t>
+  </si>
+  <si>
+    <t>To provide a comprehensive guide for designing UAV swarm experiments, including the selection of appropriate simulation platforms and the formulation of specific objectives. The paper aims to validate the resilience and performance of UAV swarm systems through simulation-based experiments.</t>
+  </si>
+  <si>
+    <t>The paper reviews the growing importance of UAV swarms in various domains, including surveillance, agriculture, military, search and rescue, and environmental monitoring. It discusses the challenges of controlling UAV swarms, such as communication delays, positioning errors, and collision avoidance. The authors highlight the use of simulation methods, particularly software-in-the-loop (SITL), for testing and validating swarm control algorithms. The paper also references foundational works on swarm robotics, distributed consensus models, and the application of swarm intelligence in adaptive routing and formation control.</t>
+  </si>
+  <si>
+    <t>To analyze the impact of positioning errors, communication delays, and swarm speed on the coordination and collision avoidance capabilities of UAV swarms in a simulated environment.</t>
+  </si>
+  <si>
+    <t>A detailed analysis of the impact of GPS positioning errors and communication delays on swarm coordination.
+Development of a leader-based control mechanism for UAV swarms.
+Simulation-based validation of swarm control algorithms using SITL.
+Identification of minimum safe distances between drones to avoid collisions under various conditions.</t>
+  </si>
+  <si>
+    <t>Algorithms: Leader-based control mechanism, collision avoidance algorithms, artificial potential fields, bio-inspired pheromone maps.
+Hardware: Ryze Tello EDU drones, Robolink CoDrones.
+Software: MATLAB UAV Toolbox, Simulink, RflySim.</t>
+  </si>
+  <si>
+    <t>MATLAB: Used for 2D swarm simulations, path planning, and formation control.
+OMNET++: Used for FANET (Flying Ad Hoc Networks) and MANET (Mobile Ad Hoc Networks) simulations.
+Webots: Used for photorealistic UAV simulations and heterogeneous swarm testing.
+CoppeliaSim: Used for swarm topology and inter-agent policy testing.
+Microsoft AirSim: Used for high-fidelity UAV simulations with weather effects.</t>
+  </si>
+  <si>
+    <t>Minimum Distance Between Drones: The minimum safe distance required to avoid collisions under different conditions.
+Swarm Speed: The maximum safe speed at which the swarm can operate without collisions.
+Positioning Accuracy: The impact of GPS positioning errors on swarm coordination.
+Communication Delays: The effect of communication delays on swarm synchronization and collision avoidance.
+Energy Efficiency: The impact of swarm speed and trajectory on fuel efficiency.
+Task Completion Time: The time taken to complete tasks such as target search and area coverage.</t>
+  </si>
+  <si>
+    <t>Leader-Based Control Model: The swarm follows a leader drone, with each drone mimicking the leader's trajectory and movements. This model ensures coherent coordination and collision avoidance within the swarm.
+Artificial Potential Fields (APF): Used for attraction and repulsion forces to maintain swarm formation.
+Pheromone Maps: Inspired by biological systems, used for target convergence and path planning.</t>
+  </si>
+  <si>
+    <t>GPS: For precise positioning and navigation.
+LiDAR: For obstacle detection and mapping.
+Fisheye Cameras: For visual data collection and target detection.
+Ultrasonic Sensors: For close-range obstacle avoidance.
+Passive Beacons: For localized positioning and drift compensation.</t>
+  </si>
+  <si>
+    <t>Positioning Errors: GPS inaccuracies can affect swarm coordination and collision avoidance.
+Communication Delays: Delays in data transmission can lead to synchronization issues and collisions.
+Swarm Speed: Higher speeds increase the risk of collisions, especially in dense formations.
+Battery Life: Limited battery capacity restricts the operational time of drones.
+Environmental Complexity: Obstacles and dynamic environments can challenge swarm coordination.
+Weather Conditions: Adverse weather (e.g., rain, fog, wind) can impact sensor performance and swarm coordination.</t>
+  </si>
+  <si>
+    <t>Formation Maintenance: Drones must maintain a specific formation (e.g., grid structure) while navigating.
+Collision Avoidance: Drones must avoid collisions with each other and obstacles.
+Speed Variation: Drones must operate at varying speeds (1–5 m/s) while maintaining formation.
+Communication Testing: The impact of communication delays (0 ms to 500 ms) on swarm coordination is tested.
+Positioning Accuracy: The effect of GPS positioning errors (0 cm, 5 cm, 50 cm, 100 cm) on swarm coordination is evaluated.
+Target Search and Rescue: Drones must locate and converge on a target (e.g., a person in distress) in a realistic environment.
+Area Coverage: Drones must efficiently cover a designated area for surveillance or data collection.</t>
+  </si>
+  <si>
+    <t>Wajeeha Nasar, Ricardo Da Silva Torres, Odd Erik Gundersen, Anniken T. Karlsen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wajeeha Nasar, Ricardo Da Silva Torres, Anniken T. Karlsen: Department of ICT and Natural Sciences, Faculty of Information Technology and Electrical Engineering, NTNU—Norwegian University of Science and Technology, Ålesund, Norway.
+Odd Erik Gundersen: Department of Computer Science, Faculty of Information Technology and Electrical Engineering, NTNU—Norwegian University of Science and Technology, Trondheim, Norway.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MDPI </t>
+  </si>
+  <si>
+    <t>ISPRS International Journal of Geo-Information</t>
+  </si>
+  <si>
+    <t>Artificial intelligence, data management, decision support, disaster management, geographical information systems, search and rescue operations, spatial analysis, systematic review</t>
+  </si>
+  <si>
+    <t>Artificial intelligence , decision support ,  search and rescue operations</t>
+  </si>
+  <si>
+    <t>Limited research on decision support systems (DSS) for search and rescue (SAR) at sea.
+Most existing studies focus on land-based SAR operations, with fewer addressing maritime or aerial SAR.
+Lack of integration of AI technologies with data management solutions for real-time decision-making in SAR.
+Few studies explore the knowledge transfer between different SAR application areas (e.g., land, sea, air).</t>
+  </si>
+  <si>
+    <t>Further research on DSS for SAR at sea to address the gap in maritime SAR operations.
+Development of AI-driven solutions for real-time decision-making in SAR, especially in complex environments.
+Exploration of knowledge transfer between different SAR domains (e.g., applying land-based solutions to maritime or aerial SAR).
+Integration of advanced data management solutions (e.g., big data, IoT, cloud computing) with AI technologies for more efficient SAR operations.
+Focus on multi-agent systems and swarm robotics for collaborative SAR tasks.</t>
+  </si>
+  <si>
+    <t>To provide a systematic literature review of the use of decision support systems (DSS), data management solutions, and artificial intelligence (AI) in search and rescue (SAR) operations.
+To identify existing solutions, analyze their contributions, and explore the potential for knowledge transfer between different SAR application areas.</t>
+  </si>
+  <si>
+    <t>The paper reviews various studies on the use of DSS, data management solutions, and AI in SAR operations.
+It highlights the integration of geographical information systems (GIS) with machine learning (ML) for land-based SAR.
+The review identifies the use of UAVs (drones), IoT, and big data in SAR operations, particularly for data acquisition and situational awareness.
+The paper also discusses the limitations of existing research, such as the lack of focus on maritime SAR and the need for more real-time decision-making solutions.</t>
+  </si>
+  <si>
+    <t>To systematize existing knowledge on the use of DSS, data management solutions, and AI in SAR processes.
+To identify research patterns, gaps, and opportunities for knowledge transfer between different SAR application areas.</t>
+  </si>
+  <si>
+    <t>A comprehensive bibliometric mapping and systematic literature review of DSS, data management, and AI in SAR.
+Identification of research gaps, particularly in maritime SAR and real-time decision-making.
+Discussion of knowledge transfer possibilities between different SAR domains.
+Insights into the use of AI technologies (e.g., ML, DL, NLP) and data management solutions (e.g., GIS, IoT, big data) in SAR operations.</t>
+  </si>
+  <si>
+    <t>Decision Support Systems (DSS): Used for decision-making and planning in SAR operations.
+Data Management Solutions: Including GIS, IoT, big data, and cloud computing for data collection, storage, and analysis.
+AI Technologies: Including machine learning (ML), deep learning (DL), natural language processing (NLP), and reinforcement learning (RL) for data analysis and decision-making.
+UAVs (Drones): Used for data acquisition and situational awareness in SAR operations.</t>
+  </si>
+  <si>
+    <t>Drone Battery Capacity : 
+Drones are used for extended missions, implying the need for efficient battery usage.
+Missions often involve harsh terrain and weather conditions, which can drain battery life faster.
+Time for Survivors:
+Time is critical in SAR operations, and drone swarms aim to reduce the time required to locate survivors.
+The faster the swarm can cover the area, the higher the chance of finding survivors in time.
+Swarm Coordination: Drones and robots need to work together efficiently, which requires robust communication and coordination algorithms.
+Environmental Challenges: Harsh terrain and weather conditions can affect both drone and robot battery life and performance.
+Autonomy: The system should be partially autonomous to reduce the cognitive load on operators</t>
+  </si>
+  <si>
+    <t>Scalability: The system must handle large numbers of robots without significant performance degradation.
+Robustness: The swarm should continue functioning even if some robots fail or run out of battery.
+Communication: Reliable communication between drones and robots is essential for coordination.
+Energy Efficiency: Algorithms must optimize energy usage to extend mission duration.
+Drone/Robot Battery:
+Energy efficiency is a key challenge, especially in remote or harsh environments where recharging is difficult.
+Algorithms like PSO and RL need to optimize energy consumption during path planning and task allocation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Environment Complexity: The system must handle both empty and cluttered environments, which can affect battery life and search time.
+Verification: Most strategies are tested in simulation, but real-world testing is needed to validate battery life and performance.
+Dynamic Environments: The system must adapt to changing conditions, which can impact battery usage and search time.
+</t>
+  </si>
+  <si>
+    <t>Communication Delays:
+Communication delays (0 ms to 500 ms) significantly impact swarm coordination and collision avoidance. Faster networks (e.g., Wi-Fi) are recommended for safe swarm operations.
+Positioning Accuracy:
+High-precision positioning (e.g., RTK GPS with 5 cm accuracy) is crucial for maintaining swarm formation and avoiding collisions, especially in close-proximity flights.
+Swarm Formation:
+Two main formations are studied:
+Grid formation with a leader drone.
+Leader-follower formation where each drone follows its predecessor.
+Formation type affects coordination, especially under delays and positioning errors.
+Collision Avoidance:
+The minimum safe distance between drones depends on speed, communication delays, and positioning errors. Advanced collision avoidance mechanisms are needed for higher speeds.
+Speed of Swarm Movement:
+Swarm speed (1 m/s to 5 m/s) impacts coordination and collision avoidance. Higher speeds require more precise control and communication.</t>
+  </si>
+  <si>
+    <t>Swarm Formation and Control:
+Swarm formations can be centralized, decentralized, or hybrid, depending on the mission requirements.
+Leader-follower models and grid-based formations are commonly used for coordination and collision avoidance.
+Artificial Potential Fields (APF) and pheromone-based techniques are used for swarm movement and target convergence.
+Communication and Network Topology:
+FANET (Flying Ad Hoc Networks) is used for inter-agent communication in UAV swarms.
+AODV (Ad Hoc On-Demand Distance Vector) is a common routing protocol for swarm communication, ensuring reliable data transmission.
+Communication delays and network strength are critical for maintaining swarm coordination and avoiding collisions.
+Simulation Platforms:
+MATLAB, CoppeliaSim, Webots, and OMNET++ are popular simulation tools for testing UAV swarm behaviors.
+Simulations allow for testing swarm behaviors in realistic environments, including weather effects like rain, fog, and wind.
+Software-in-the-loop (SITL) simulations are used to validate swarm control algorithms before real-world deployment.
+Heterogeneous Swarms:
+Heterogeneous swarms (e.g., UAVs and UGVs) can improve mission efficiency by leveraging the unique capabilities of each agent.
+For example, UAVs can provide aerial surveillance, while UGVs can handle ground-based tasks like landing platforms or obstacle detection.
+Collision Avoidance:
+Minimum distance thresholds between drones are set to avoid collisions, depending on swarm speed, communication delays, and positioning accuracy.
+Low-tolerance controllers ensure minimal intrusion but require more computational power, while high-tolerance controllers are less computationally intensive but risk collisions.
+Search and Rescue (SAR):
+UAV swarms can be deployed in grid-based or randomized patterns to cover large areas efficiently.
+Targeted deployment focuses on critical areas, while adaptive deployment adjusts based on real-time data.
+Swarms can use vision sensors, LiDAR, and ultrasonic sensors to detect survivors and obstacles.
+Weather Effects:
+Weather conditions like rain, fog, and wind can impact UAV performance, sensor accuracy, and swarm coordination.
+Simulations incorporate weather effects to test swarm resilience in adverse conditions.
+Simulation-to-Real-World Integration:
+Hardware-in-the-loop (HIL) experiments bridge the gap between simulation and real-world testing.
+Platforms like Ryze Tello and Robolink Codrone allow for real-world testing of swarm behaviors developed in simulations.</t>
   </si>
 </sst>
 </file>
@@ -1748,7 +2245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1817,6 +2314,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1928,50 +2428,6 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>2201142</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>275360</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>7391400</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>3128862</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFD7C1BC-BCB7-2B4C-93EC-84EEAB3EE34F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="44244492" y="2789960"/>
-          <a:ext cx="5190258" cy="2853502"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>15</xdr:col>
       <xdr:colOff>3047418</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>34160</xdr:rowOff>
@@ -1996,7 +2452,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2040,7 +2496,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2084,7 +2540,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2128,7 +2584,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
         <a:srcRect b="4242"/>
         <a:stretch/>
       </xdr:blipFill>
@@ -2171,7 +2627,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2215,7 +2671,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2259,7 +2715,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2303,7 +2759,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2347,7 +2803,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2391,7 +2847,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2435,7 +2891,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2444,6 +2900,182 @@
         <a:xfrm>
           <a:off x="71579922" y="41817234"/>
           <a:ext cx="1765855" cy="2711849"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>331306</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>59636</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>5091564</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>5141266</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C81B758D-6008-DAFB-7C21-24E5567B301E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="69547410" y="58143914"/>
+          <a:ext cx="4760258" cy="5081630"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>116541</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>89647</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>2542220</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>2097741</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9D15E89-E026-B42E-BDEA-09FD4212C866}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="69324070" y="63362541"/>
+          <a:ext cx="2425679" cy="2008094"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>2752165</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>129081</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>4900344</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>2120371</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED4ECD55-DC43-225B-73BB-23B753936FA6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="71959694" y="63401975"/>
+          <a:ext cx="2148179" cy="1991290"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>1325880</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>320041</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>8580992</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>3353997</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FC230EF-F605-43A0-3895-6FAEB6F95FEE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="70538340" y="65973961"/>
+          <a:ext cx="7255112" cy="3033956"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2496,7 +3128,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="7">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="8">
   <rv s="0">
     <v>0</v>
     <v>5</v>
@@ -2525,6 +3157,10 @@
     <v>6</v>
     <v>5</v>
   </rv>
+  <rv s="0">
+    <v>7</v>
+    <v>5</v>
+  </rv>
 </rvData>
 </file>
 
@@ -2546,6 +3182,7 @@
   <rel r:id="rId5"/>
   <rel r:id="rId6"/>
   <rel r:id="rId7"/>
+  <rel r:id="rId8"/>
 </richValueRels>
 </file>
 
@@ -2866,11 +3503,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16033D29-535B-46C8-9A04-5BEF5D9655C0}">
-  <dimension ref="A1:W26"/>
+  <dimension ref="A1:Z45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="V1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Y26" sqref="Y26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2898,9 +3535,12 @@
     <col min="21" max="21" width="22.6640625" customWidth="1"/>
     <col min="22" max="22" width="41" customWidth="1"/>
     <col min="23" max="23" width="43.88671875" customWidth="1"/>
+    <col min="24" max="24" width="67.5546875" customWidth="1"/>
+    <col min="25" max="25" width="73" customWidth="1"/>
+    <col min="26" max="26" width="60.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="24" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:26" ht="24" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -2911,22 +3551,22 @@
         <v>1</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="F1" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="J1" s="10" t="s">
         <v>3</v>
@@ -2944,10 +3584,10 @@
         <v>7</v>
       </c>
       <c r="O1" s="10" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="P1" s="10" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="Q1" s="10" t="s">
         <v>16</v>
@@ -2965,13 +3605,22 @@
         <v>19</v>
       </c>
       <c r="V1" s="10" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
       <c r="W1" s="11" t="s">
-        <v>30</v>
+        <v>24</v>
+      </c>
+      <c r="X1" s="11" t="s">
+        <v>340</v>
+      </c>
+      <c r="Y1" s="11" t="s">
+        <v>341</v>
+      </c>
+      <c r="Z1" s="11" t="s">
+        <v>342</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="399.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" ht="399.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -2982,22 +3631,22 @@
         <v>10</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>8</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="J2" s="14" t="s">
         <v>11</v>
@@ -3009,7 +3658,7 @@
         <v>13</v>
       </c>
       <c r="M2" s="26" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
       <c r="N2" s="14" t="s">
         <v>14</v>
@@ -3019,13 +3668,13 @@
       </c>
       <c r="P2" s="15"/>
       <c r="Q2" s="14" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="R2" s="14" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="S2" s="26" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="T2" s="14" t="s">
         <v>21</v>
@@ -3034,80 +3683,88 @@
         <v>5</v>
       </c>
       <c r="V2" s="13" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="W2" s="13" t="s">
-        <v>49</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="X2" s="13"/>
+      <c r="Y2" s="13"/>
+      <c r="Z2" s="13"/>
     </row>
-    <row r="3" spans="1:23" ht="247.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" ht="247.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16">
         <v>2</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="17">
+        <v>2023</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>413</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>414</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>415</v>
+      </c>
+      <c r="F3" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>24</v>
-      </c>
       <c r="G3" s="14" t="s">
-        <v>328</v>
+        <v>416</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>89</v>
+        <v>418</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>88</v>
+        <v>417</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="13"/>
+        <v>419</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>420</v>
+      </c>
       <c r="L3" s="13" t="s">
-        <v>26</v>
+        <v>421</v>
       </c>
       <c r="M3" s="27" t="s">
-        <v>325</v>
+        <v>422</v>
       </c>
       <c r="N3" s="13" t="s">
-        <v>29</v>
+        <v>423</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>329</v>
+        <v>424</v>
       </c>
       <c r="P3" s="20"/>
       <c r="Q3" s="13" t="s">
-        <v>28</v>
+        <v>425</v>
       </c>
       <c r="R3" s="19" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="S3" s="27" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="T3" s="13" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="U3" s="14">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="V3" s="14" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="W3" s="14" t="s">
-        <v>49</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="X3" s="14"/>
+      <c r="Y3" s="14"/>
+      <c r="Z3" s="14"/>
     </row>
-    <row r="4" spans="1:23" ht="242.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" ht="242.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="21">
         <v>3</v>
       </c>
@@ -3115,66 +3772,69 @@
         <v>2023</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="F4" s="14" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="L4" s="14" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
       <c r="N4" s="14" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="O4" s="14" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="P4" s="14"/>
       <c r="Q4" s="14" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="R4" s="14" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="S4" s="14"/>
       <c r="T4" s="14" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="U4" s="14">
         <v>4</v>
       </c>
       <c r="V4" s="14" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="W4" s="14" t="s">
-        <v>41</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="X4" s="14"/>
+      <c r="Y4" s="14"/>
+      <c r="Z4" s="14"/>
     </row>
-    <row r="5" spans="1:23" ht="151.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" ht="151.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="21">
         <v>4</v>
       </c>
@@ -3182,66 +3842,69 @@
         <v>2022</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D5" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="H5" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="E5" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>74</v>
-      </c>
       <c r="I5" s="14" t="s">
-        <v>330</v>
+        <v>317</v>
       </c>
       <c r="J5" s="14" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="K5" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="L5" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="M5" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="L5" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="M5" s="14" t="s">
-        <v>51</v>
-      </c>
       <c r="N5" s="14" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="O5" s="14" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="P5" s="14"/>
       <c r="Q5" s="14" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="R5" s="14" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="S5" s="14"/>
       <c r="T5" s="14" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="U5" s="14">
         <v>4</v>
       </c>
       <c r="V5" s="14" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="W5" s="14" t="s">
-        <v>49</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="X5" s="14"/>
+      <c r="Y5" s="14"/>
+      <c r="Z5" s="14"/>
     </row>
-    <row r="6" spans="1:23" ht="277.8" customHeight="1" x14ac:dyDescent="1.2">
+    <row r="6" spans="1:26" ht="277.8" customHeight="1" x14ac:dyDescent="1.2">
       <c r="A6" s="21">
         <v>5</v>
       </c>
@@ -3249,68 +3912,71 @@
         <v>2023</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="J6" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="L6" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="M6" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="K6" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="L6" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="M6" s="14" t="s">
-        <v>61</v>
-      </c>
       <c r="N6" s="14" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="O6" s="14" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="P6" s="14" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
       <c r="Q6" s="23" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="R6" s="23" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="S6" s="14"/>
       <c r="T6" s="14" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="U6" s="14">
         <v>2</v>
       </c>
       <c r="V6" s="14" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="W6" s="14" t="s">
-        <v>62</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="X6" s="14"/>
+      <c r="Y6" s="14"/>
+      <c r="Z6" s="14"/>
     </row>
-    <row r="7" spans="1:23" ht="177.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" ht="177.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="21">
         <v>6</v>
       </c>
@@ -3318,70 +3984,73 @@
         <v>2021</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>331</v>
+        <v>318</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>332</v>
+        <v>319</v>
       </c>
       <c r="L7" s="14" t="s">
-        <v>333</v>
+        <v>320</v>
       </c>
       <c r="M7" s="14" t="s">
-        <v>334</v>
+        <v>321</v>
       </c>
       <c r="N7" s="14" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="O7" s="28" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="P7" s="14" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
       <c r="Q7" s="14" t="s">
-        <v>335</v>
+        <v>322</v>
       </c>
       <c r="R7" s="14" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="S7" s="14" t="s">
-        <v>336</v>
+        <v>323</v>
       </c>
       <c r="T7" s="14" t="s">
-        <v>337</v>
+        <v>324</v>
       </c>
       <c r="U7" s="14">
         <v>4</v>
       </c>
       <c r="V7" s="14" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="W7" s="14" t="s">
-        <v>62</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="X7" s="14"/>
+      <c r="Y7" s="14"/>
+      <c r="Z7" s="14"/>
     </row>
-    <row r="8" spans="1:23" ht="157.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" ht="157.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="21">
         <v>7</v>
       </c>
@@ -3389,68 +4058,71 @@
         <v>2020</v>
       </c>
       <c r="C8" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="K8" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="L8" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="M8" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="N8" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="O8" s="26" t="s">
         <v>99</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="H8" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="I8" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="J8" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="K8" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="L8" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="M8" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="N8" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="O8" s="26" t="s">
-        <v>109</v>
       </c>
       <c r="P8" s="14"/>
       <c r="Q8" s="14" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="R8" s="14" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="S8" s="14" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="T8" s="14" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="U8" s="14">
         <v>5</v>
       </c>
       <c r="V8" s="14" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="W8" s="14" t="s">
-        <v>49</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="X8" s="14"/>
+      <c r="Y8" s="14"/>
+      <c r="Z8" s="14"/>
     </row>
-    <row r="9" spans="1:23" ht="159" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" ht="159" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="21">
         <v>8</v>
       </c>
@@ -3458,66 +4130,69 @@
         <v>2021</v>
       </c>
       <c r="C9" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="J9" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="K9" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="L9" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="M9" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="N9" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="O9" s="14" t="s">
         <v>117</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="H9" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="I9" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="J9" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="K9" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="L9" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="M9" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="N9" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="O9" s="14" t="s">
-        <v>127</v>
       </c>
       <c r="P9" s="14"/>
       <c r="Q9" s="14" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="R9" s="14" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="S9" s="14"/>
       <c r="T9" s="14" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="U9" s="14">
         <v>5</v>
       </c>
       <c r="V9" s="14" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="W9" s="14" t="s">
-        <v>49</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="X9" s="14"/>
+      <c r="Y9" s="14"/>
+      <c r="Z9" s="14"/>
     </row>
-    <row r="10" spans="1:23" ht="230.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" ht="230.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="21">
         <v>9</v>
       </c>
@@ -3525,66 +4200,69 @@
         <v>2023</v>
       </c>
       <c r="C10" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="J10" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="K10" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="L10" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="M10" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="N10" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="O10" s="14" t="s">
         <v>132</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="H10" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="I10" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="J10" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="K10" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="L10" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="M10" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="N10" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="O10" s="14" t="s">
-        <v>142</v>
       </c>
       <c r="P10" s="14"/>
       <c r="Q10" s="14" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="R10" s="14" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="S10" s="14"/>
       <c r="T10" s="14" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="U10" s="14">
         <v>5</v>
       </c>
       <c r="V10" s="14" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="W10" s="14" t="s">
-        <v>145</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="X10" s="14"/>
+      <c r="Y10" s="14"/>
+      <c r="Z10" s="14"/>
     </row>
-    <row r="11" spans="1:23" ht="240.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" ht="240.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="21">
         <v>10</v>
       </c>
@@ -3592,68 +4270,71 @@
         <v>2020</v>
       </c>
       <c r="C11" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="J11" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="K11" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="L11" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="M11" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="N11" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="O11" s="14" t="s">
         <v>147</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="G11" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="H11" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="I11" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="J11" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="K11" s="14" t="s">
-        <v>153</v>
-      </c>
-      <c r="L11" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="M11" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="N11" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="O11" s="14" t="s">
-        <v>157</v>
       </c>
       <c r="P11" s="14"/>
       <c r="Q11" s="6" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="R11" s="14" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="S11" s="14" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="T11" s="14" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="U11" s="24">
         <v>4</v>
       </c>
       <c r="V11" s="14" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="W11" s="14" t="s">
-        <v>162</v>
-      </c>
+        <v>152</v>
+      </c>
+      <c r="X11" s="14"/>
+      <c r="Y11" s="14"/>
+      <c r="Z11" s="14"/>
     </row>
-    <row r="12" spans="1:23" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A12" s="21">
         <v>11</v>
       </c>
@@ -3661,68 +4342,71 @@
         <v>2021</v>
       </c>
       <c r="C12" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="J12" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="K12" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="L12" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="M12" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="N12" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="O12" s="14" t="s">
         <v>163</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="H12" s="14" t="s">
-        <v>167</v>
-      </c>
-      <c r="I12" s="14" t="s">
-        <v>166</v>
-      </c>
-      <c r="J12" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="K12" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="L12" s="14" t="s">
-        <v>170</v>
-      </c>
-      <c r="M12" s="14" t="s">
-        <v>171</v>
-      </c>
-      <c r="N12" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="O12" s="14" t="s">
-        <v>173</v>
       </c>
       <c r="P12" s="14"/>
       <c r="Q12" s="5" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="R12" s="14" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="S12" s="14" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="T12" s="14" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="U12" s="14">
         <v>5</v>
       </c>
       <c r="V12" s="14" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="W12" s="14" t="s">
-        <v>177</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="X12" s="14"/>
+      <c r="Y12" s="14"/>
+      <c r="Z12" s="14"/>
     </row>
-    <row r="13" spans="1:23" ht="159" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:26" ht="159" x14ac:dyDescent="0.35">
       <c r="A13" s="21">
         <v>12</v>
       </c>
@@ -3730,68 +4414,71 @@
         <v>2020</v>
       </c>
       <c r="C13" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="I13" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="J13" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="K13" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="L13" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="M13" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="N13" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="O13" s="14" t="s">
         <v>179</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>180</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13" s="14" t="s">
-        <v>181</v>
-      </c>
-      <c r="H13" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="I13" s="14" t="s">
-        <v>182</v>
-      </c>
-      <c r="J13" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="K13" s="14" t="s">
-        <v>185</v>
-      </c>
-      <c r="L13" s="14" t="s">
-        <v>186</v>
-      </c>
-      <c r="M13" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="N13" s="14" t="s">
-        <v>188</v>
-      </c>
-      <c r="O13" s="14" t="s">
-        <v>189</v>
       </c>
       <c r="P13" s="14"/>
       <c r="Q13" s="6" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="R13" s="14" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="S13" s="14" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="T13" s="14" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="U13" s="14">
         <v>3</v>
       </c>
       <c r="V13" s="14" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="W13" s="14" t="s">
-        <v>193</v>
-      </c>
+        <v>183</v>
+      </c>
+      <c r="X13" s="14"/>
+      <c r="Y13" s="14"/>
+      <c r="Z13" s="14"/>
     </row>
-    <row r="14" spans="1:23" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A14" s="21">
         <v>13</v>
       </c>
@@ -3799,70 +4486,73 @@
         <v>2020</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="J14" s="14" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="K14" s="14" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="L14" s="14" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="M14" s="14" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="N14" s="14" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="O14" s="14" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="P14" s="14" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
       <c r="Q14" s="14" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="R14" s="14" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="S14" s="14" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="T14" s="14" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="U14" s="14">
         <v>3</v>
       </c>
       <c r="V14" s="14" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="W14" s="14" t="s">
-        <v>49</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="X14" s="14"/>
+      <c r="Y14" s="14"/>
+      <c r="Z14" s="14"/>
     </row>
-    <row r="15" spans="1:23" ht="181.8" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:26" ht="181.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="21">
         <v>14</v>
       </c>
@@ -3870,68 +4560,71 @@
         <v>2021</v>
       </c>
       <c r="C15" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="I15" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="J15" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="K15" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="L15" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="M15" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="N15" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="O15" s="14" t="s">
         <v>207</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>208</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="G15" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="H15" s="14" t="s">
-        <v>211</v>
-      </c>
-      <c r="I15" s="14" t="s">
-        <v>210</v>
-      </c>
-      <c r="J15" s="14" t="s">
-        <v>212</v>
-      </c>
-      <c r="K15" s="14" t="s">
-        <v>213</v>
-      </c>
-      <c r="L15" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="M15" s="14" t="s">
-        <v>215</v>
-      </c>
-      <c r="N15" s="14" t="s">
-        <v>216</v>
-      </c>
-      <c r="O15" s="14" t="s">
-        <v>217</v>
       </c>
       <c r="P15" s="14"/>
       <c r="Q15" s="14" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="R15" s="14" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="S15" s="14" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="T15" s="14" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="U15" s="14">
         <v>4</v>
       </c>
       <c r="V15" s="14" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="W15" s="14" t="s">
-        <v>222</v>
-      </c>
+        <v>212</v>
+      </c>
+      <c r="X15" s="14"/>
+      <c r="Y15" s="14"/>
+      <c r="Z15" s="14"/>
     </row>
-    <row r="16" spans="1:23" ht="259.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" ht="259.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="21">
         <v>15</v>
       </c>
@@ -3939,70 +4632,73 @@
         <v>2020</v>
       </c>
       <c r="C16" s="22" t="s">
+        <v>213</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="I16" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="J16" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="K16" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="L16" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="M16" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="N16" s="14" t="s">
         <v>223</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="O16" s="14" t="s">
         <v>224</v>
-      </c>
-      <c r="E16" s="19" t="s">
-        <v>225</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="G16" s="14" t="s">
-        <v>226</v>
-      </c>
-      <c r="H16" s="14" t="s">
-        <v>228</v>
-      </c>
-      <c r="I16" s="14" t="s">
-        <v>227</v>
-      </c>
-      <c r="J16" s="14" t="s">
-        <v>229</v>
-      </c>
-      <c r="K16" s="14" t="s">
-        <v>230</v>
-      </c>
-      <c r="L16" s="14" t="s">
-        <v>231</v>
-      </c>
-      <c r="M16" s="14" t="s">
-        <v>232</v>
-      </c>
-      <c r="N16" s="14" t="s">
-        <v>233</v>
-      </c>
-      <c r="O16" s="14" t="s">
-        <v>234</v>
       </c>
       <c r="P16" s="14" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
       <c r="Q16" s="14" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="R16" s="14" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="S16" s="14" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="T16" s="14" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="U16" s="14">
         <v>4</v>
       </c>
       <c r="V16" s="14" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="W16" s="14" t="s">
-        <v>239</v>
-      </c>
+        <v>229</v>
+      </c>
+      <c r="X16" s="14"/>
+      <c r="Y16" s="14"/>
+      <c r="Z16" s="14"/>
     </row>
-    <row r="17" spans="1:23" ht="159" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:26" ht="159" x14ac:dyDescent="0.35">
       <c r="A17" s="21">
         <v>16</v>
       </c>
@@ -4010,68 +4706,73 @@
         <v>2021</v>
       </c>
       <c r="C17" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>233</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="I17" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="J17" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="K17" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="L17" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="M17" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="N17" s="14" t="s">
         <v>240</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="O17" s="14" t="s">
         <v>241</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="P17" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q17" s="14" t="s">
         <v>242</v>
       </c>
-      <c r="F17" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="G17" s="14" t="s">
+      <c r="R17" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="S17" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="T17" s="14" t="s">
         <v>243</v>
-      </c>
-      <c r="H17" s="14" t="s">
-        <v>245</v>
-      </c>
-      <c r="I17" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="J17" s="14" t="s">
-        <v>246</v>
-      </c>
-      <c r="K17" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="L17" s="14" t="s">
-        <v>248</v>
-      </c>
-      <c r="M17" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="N17" s="14" t="s">
-        <v>250</v>
-      </c>
-      <c r="O17" s="14" t="s">
-        <v>251</v>
-      </c>
-      <c r="P17" s="14"/>
-      <c r="Q17" s="14" t="s">
-        <v>252</v>
-      </c>
-      <c r="R17" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="S17" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="T17" s="14" t="s">
-        <v>253</v>
       </c>
       <c r="U17" s="14">
         <v>5</v>
       </c>
       <c r="V17" s="14" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="W17" s="14" t="s">
-        <v>49</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="X17" s="14"/>
+      <c r="Y17" s="14"/>
+      <c r="Z17" s="14"/>
     </row>
-    <row r="18" spans="1:23" ht="240" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:26" ht="240" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="21">
         <v>17</v>
       </c>
@@ -4079,70 +4780,73 @@
         <v>2021</v>
       </c>
       <c r="C18" s="25" t="s">
+        <v>245</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="I18" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="J18" s="14" t="s">
+        <v>252</v>
+      </c>
+      <c r="K18" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="L18" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="M18" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="D18" s="13" t="s">
-        <v>258</v>
-      </c>
-      <c r="E18" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="G18" s="14" t="s">
-        <v>259</v>
-      </c>
-      <c r="H18" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="I18" s="14" t="s">
-        <v>260</v>
-      </c>
-      <c r="J18" s="14" t="s">
-        <v>262</v>
-      </c>
-      <c r="K18" s="14" t="s">
-        <v>263</v>
-      </c>
-      <c r="L18" s="14" t="s">
-        <v>264</v>
-      </c>
-      <c r="M18" s="14" t="s">
-        <v>265</v>
-      </c>
       <c r="N18" s="7" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="O18" s="14" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="P18" s="14" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
       <c r="Q18" s="14" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="R18" s="14" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="S18" s="14" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="T18" s="14" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="U18" s="14">
         <v>5</v>
       </c>
       <c r="V18" s="14" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="W18" s="14" t="s">
-        <v>49</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="X18" s="14"/>
+      <c r="Y18" s="14"/>
+      <c r="Z18" s="14"/>
     </row>
-    <row r="19" spans="1:23" ht="159" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:26" ht="159" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="21">
         <v>18</v>
       </c>
@@ -4150,70 +4854,73 @@
         <v>2021</v>
       </c>
       <c r="C19" s="25" t="s">
+        <v>264</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>265</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="I19" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="J19" s="14" t="s">
+        <v>270</v>
+      </c>
+      <c r="K19" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="L19" s="14" t="s">
+        <v>272</v>
+      </c>
+      <c r="M19" s="14" t="s">
+        <v>273</v>
+      </c>
+      <c r="N19" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="O19" s="8" t="s">
         <v>275</v>
-      </c>
-      <c r="E19" s="19" t="s">
-        <v>276</v>
-      </c>
-      <c r="F19" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="G19" s="14" t="s">
-        <v>277</v>
-      </c>
-      <c r="H19" s="14" t="s">
-        <v>279</v>
-      </c>
-      <c r="I19" s="14" t="s">
-        <v>278</v>
-      </c>
-      <c r="J19" s="14" t="s">
-        <v>280</v>
-      </c>
-      <c r="K19" s="14" t="s">
-        <v>281</v>
-      </c>
-      <c r="L19" s="14" t="s">
-        <v>282</v>
-      </c>
-      <c r="M19" s="14" t="s">
-        <v>283</v>
-      </c>
-      <c r="N19" s="14" t="s">
-        <v>284</v>
-      </c>
-      <c r="O19" s="8" t="s">
-        <v>285</v>
       </c>
       <c r="P19" s="14" t="e" vm="6">
         <v>#VALUE!</v>
       </c>
       <c r="Q19" s="14" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="R19" s="14" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="S19" s="14" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="T19" s="14" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="U19" s="14">
         <v>5</v>
       </c>
       <c r="V19" s="14" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="W19" s="14" t="s">
-        <v>291</v>
-      </c>
+        <v>281</v>
+      </c>
+      <c r="X19" s="14"/>
+      <c r="Y19" s="14"/>
+      <c r="Z19" s="14"/>
     </row>
-    <row r="20" spans="1:23" ht="198.6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:26" ht="198.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="21">
         <v>19</v>
       </c>
@@ -4221,70 +4928,73 @@
         <v>2020</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="D20" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="E20" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="H20" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="I20" s="14" t="s">
+        <v>285</v>
+      </c>
+      <c r="J20" s="14" t="s">
+        <v>287</v>
+      </c>
+      <c r="K20" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="L20" s="14" t="s">
+        <v>289</v>
+      </c>
+      <c r="M20" s="14" t="s">
+        <v>290</v>
+      </c>
+      <c r="N20" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="O20" s="8" t="s">
         <v>292</v>
-      </c>
-      <c r="E20" s="25" t="s">
-        <v>225</v>
-      </c>
-      <c r="F20" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="G20" s="14" t="s">
-        <v>294</v>
-      </c>
-      <c r="H20" s="14" t="s">
-        <v>296</v>
-      </c>
-      <c r="I20" s="14" t="s">
-        <v>295</v>
-      </c>
-      <c r="J20" s="14" t="s">
-        <v>297</v>
-      </c>
-      <c r="K20" s="14" t="s">
-        <v>298</v>
-      </c>
-      <c r="L20" s="14" t="s">
-        <v>299</v>
-      </c>
-      <c r="M20" s="14" t="s">
-        <v>300</v>
-      </c>
-      <c r="N20" s="14" t="s">
-        <v>301</v>
-      </c>
-      <c r="O20" s="8" t="s">
-        <v>302</v>
       </c>
       <c r="P20" s="14" t="e" vm="7">
         <v>#VALUE!</v>
       </c>
       <c r="Q20" s="14" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="R20" s="14" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
       <c r="S20" s="14" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="T20" s="14" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="U20" s="14">
         <v>4</v>
       </c>
       <c r="V20" s="14" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="W20" s="14" t="s">
-        <v>308</v>
-      </c>
+        <v>298</v>
+      </c>
+      <c r="X20" s="14"/>
+      <c r="Y20" s="14"/>
+      <c r="Z20" s="14"/>
     </row>
-    <row r="21" spans="1:23" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:26" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A21" s="21">
         <v>20</v>
       </c>
@@ -4292,170 +5002,997 @@
         <v>2021</v>
       </c>
       <c r="C21" s="22" t="s">
+        <v>299</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>300</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>301</v>
+      </c>
+      <c r="H21" s="14" t="s">
+        <v>303</v>
+      </c>
+      <c r="I21" s="14" t="s">
+        <v>302</v>
+      </c>
+      <c r="J21" s="14" t="s">
+        <v>304</v>
+      </c>
+      <c r="K21" s="14" t="s">
+        <v>305</v>
+      </c>
+      <c r="L21" s="14" t="s">
+        <v>306</v>
+      </c>
+      <c r="M21" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="N21" s="14" t="s">
+        <v>308</v>
+      </c>
+      <c r="O21" s="8" t="s">
         <v>309</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="P21" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q21" s="14" t="s">
         <v>310</v>
       </c>
-      <c r="E21" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="G21" s="14" t="s">
+      <c r="R21" s="14" t="s">
         <v>311</v>
       </c>
-      <c r="H21" s="14" t="s">
-        <v>313</v>
-      </c>
-      <c r="I21" s="14" t="s">
+      <c r="S21" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="T21" s="14" t="s">
         <v>312</v>
-      </c>
-      <c r="J21" s="14" t="s">
-        <v>314</v>
-      </c>
-      <c r="K21" s="14" t="s">
-        <v>315</v>
-      </c>
-      <c r="L21" s="14" t="s">
-        <v>316</v>
-      </c>
-      <c r="M21" s="14" t="s">
-        <v>317</v>
-      </c>
-      <c r="N21" s="14" t="s">
-        <v>318</v>
-      </c>
-      <c r="O21" s="8" t="s">
-        <v>319</v>
-      </c>
-      <c r="P21" s="14"/>
-      <c r="Q21" s="14" t="s">
-        <v>320</v>
-      </c>
-      <c r="R21" s="14" t="s">
-        <v>321</v>
-      </c>
-      <c r="S21" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="T21" s="14" t="s">
-        <v>322</v>
       </c>
       <c r="U21" s="14">
         <v>5</v>
       </c>
       <c r="V21" s="14" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="W21" s="14" t="s">
-        <v>49</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="X21" s="14"/>
+      <c r="Y21" s="14"/>
+      <c r="Z21" s="14"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A22" s="3"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
-      <c r="P22" s="2"/>
-      <c r="Q22" s="2"/>
-      <c r="R22" s="2"/>
-      <c r="S22" s="2"/>
-      <c r="T22" s="2"/>
-      <c r="U22" s="2"/>
-      <c r="V22" s="2"/>
-      <c r="W22" s="2"/>
+    <row r="22" spans="1:26" ht="287.39999999999998" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>326</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>327</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="O22" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="P22" s="2" t="e" vm="8">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q22" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="R22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="S22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T22" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="U22" s="2">
+        <v>5</v>
+      </c>
+      <c r="V22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="W22" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="X22" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="Y22" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="Z22" s="2" t="s">
+        <v>426</v>
+      </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A23" s="3"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-      <c r="O23" s="2"/>
-      <c r="P23" s="2"/>
-      <c r="Q23" s="2"/>
-      <c r="R23" s="2"/>
-      <c r="S23" s="2"/>
-      <c r="T23" s="2"/>
-      <c r="U23" s="2"/>
-      <c r="V23" s="2"/>
-      <c r="W23" s="2"/>
+    <row r="23" spans="1:26" ht="247.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="N23" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="O23" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="P23" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q23" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="R23" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="S23" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T23" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="U23" s="2">
+        <v>5</v>
+      </c>
+      <c r="V23" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="W23" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="X23" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="Y23" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="Z23" s="2" t="s">
+        <v>427</v>
+      </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A24" s="3"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
-      <c r="O24" s="2"/>
+    <row r="24" spans="1:26" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="D24" s="29" t="s">
+        <v>361</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="O24" s="2" t="s">
+        <v>370</v>
+      </c>
       <c r="P24" s="2"/>
-      <c r="Q24" s="2"/>
-      <c r="R24" s="2"/>
-      <c r="S24" s="2"/>
-      <c r="T24" s="2"/>
-      <c r="U24" s="2"/>
-      <c r="V24" s="2"/>
-      <c r="W24" s="2"/>
+      <c r="Q24" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="R24" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="S24" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T24" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="U24" s="2">
+        <v>4</v>
+      </c>
+      <c r="V24" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="W24" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="X24" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="Y24" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="Z24" s="2" t="s">
+        <v>428</v>
+      </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A25" s="3"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
-      <c r="O25" s="2"/>
+    <row r="25" spans="1:26" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>378</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>386</v>
+      </c>
       <c r="P25" s="2"/>
-      <c r="Q25" s="2"/>
-      <c r="R25" s="2"/>
-      <c r="S25" s="2"/>
-      <c r="T25" s="2"/>
-      <c r="U25" s="2"/>
-      <c r="V25" s="2"/>
-      <c r="W25" s="2"/>
+      <c r="Q25" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="R25" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="S25" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T25" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="U25" s="2">
+        <v>4</v>
+      </c>
+      <c r="V25" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="W25" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="X25" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="Y25" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="Z25" s="2" t="s">
+        <v>429</v>
+      </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
+    <row r="26" spans="1:26" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="D26" s="29" t="s">
+        <v>395</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="O26" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="R26" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="S26" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T26" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="U26" s="2">
+        <v>5</v>
+      </c>
+      <c r="V26" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="W26" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="X26" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="Y26" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="Z26" s="2" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A27" s="3"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2"/>
+      <c r="U27" s="2"/>
+      <c r="V27" s="2"/>
+      <c r="W27" s="2"/>
+      <c r="X27" s="2"/>
+      <c r="Y27" s="2"/>
+      <c r="Z27" s="2"/>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A28" s="3"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2"/>
+      <c r="S28" s="2"/>
+      <c r="T28" s="2"/>
+      <c r="U28" s="2"/>
+      <c r="V28" s="2"/>
+      <c r="W28" s="2"/>
+      <c r="X28" s="2"/>
+      <c r="Y28" s="2"/>
+      <c r="Z28" s="2"/>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A29" s="3"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="2"/>
+      <c r="S29" s="2"/>
+      <c r="T29" s="2"/>
+      <c r="U29" s="2"/>
+      <c r="V29" s="2"/>
+      <c r="W29" s="2"/>
+      <c r="X29" s="2"/>
+      <c r="Y29" s="2"/>
+      <c r="Z29" s="2"/>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A30" s="3"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="2"/>
+      <c r="S30" s="2"/>
+      <c r="T30" s="2"/>
+      <c r="U30" s="2"/>
+      <c r="V30" s="2"/>
+      <c r="W30" s="2"/>
+      <c r="X30" s="2"/>
+      <c r="Y30" s="2"/>
+      <c r="Z30" s="2"/>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A31" s="3"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+      <c r="R31" s="2"/>
+      <c r="S31" s="2"/>
+      <c r="T31" s="2"/>
+      <c r="U31" s="2"/>
+      <c r="V31" s="2"/>
+      <c r="W31" s="2"/>
+      <c r="X31" s="2"/>
+      <c r="Y31" s="2"/>
+      <c r="Z31" s="2"/>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A32" s="3"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
+      <c r="R32" s="2"/>
+      <c r="S32" s="2"/>
+      <c r="T32" s="2"/>
+      <c r="U32" s="2"/>
+      <c r="V32" s="2"/>
+      <c r="W32" s="2"/>
+      <c r="X32" s="2"/>
+      <c r="Y32" s="2"/>
+      <c r="Z32" s="2"/>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A33" s="3"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
+      <c r="R33" s="2"/>
+      <c r="S33" s="2"/>
+      <c r="T33" s="2"/>
+      <c r="U33" s="2"/>
+      <c r="V33" s="2"/>
+      <c r="W33" s="2"/>
+      <c r="X33" s="2"/>
+      <c r="Y33" s="2"/>
+      <c r="Z33" s="2"/>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A34" s="3"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
+      <c r="R34" s="2"/>
+      <c r="S34" s="2"/>
+      <c r="T34" s="2"/>
+      <c r="U34" s="2"/>
+      <c r="V34" s="2"/>
+      <c r="W34" s="2"/>
+      <c r="X34" s="2"/>
+      <c r="Y34" s="2"/>
+      <c r="Z34" s="2"/>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A35" s="3"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="2"/>
+      <c r="R35" s="2"/>
+      <c r="S35" s="2"/>
+      <c r="T35" s="2"/>
+      <c r="U35" s="2"/>
+      <c r="V35" s="2"/>
+      <c r="W35" s="2"/>
+      <c r="X35" s="2"/>
+      <c r="Y35" s="2"/>
+      <c r="Z35" s="2"/>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A36" s="3"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="29"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2"/>
+      <c r="R36" s="2"/>
+      <c r="S36" s="2"/>
+      <c r="T36" s="2"/>
+      <c r="U36" s="2"/>
+      <c r="V36" s="2"/>
+      <c r="W36" s="2"/>
+      <c r="X36" s="2"/>
+      <c r="Y36" s="2"/>
+      <c r="Z36" s="2"/>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A37" s="3"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="29"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="2"/>
+      <c r="R37" s="2"/>
+      <c r="S37" s="2"/>
+      <c r="T37" s="2"/>
+      <c r="U37" s="2"/>
+      <c r="V37" s="2"/>
+      <c r="W37" s="2"/>
+      <c r="X37" s="2"/>
+      <c r="Y37" s="2"/>
+      <c r="Z37" s="2"/>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A38" s="3"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="29"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="2"/>
+      <c r="R38" s="2"/>
+      <c r="S38" s="2"/>
+      <c r="T38" s="2"/>
+      <c r="U38" s="2"/>
+      <c r="V38" s="2"/>
+      <c r="W38" s="2"/>
+      <c r="X38" s="2"/>
+      <c r="Y38" s="2"/>
+      <c r="Z38" s="2"/>
+    </row>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A39" s="3"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="29"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2"/>
+      <c r="Q39" s="2"/>
+      <c r="R39" s="2"/>
+      <c r="S39" s="2"/>
+      <c r="T39" s="2"/>
+      <c r="U39" s="2"/>
+      <c r="V39" s="2"/>
+      <c r="W39" s="2"/>
+      <c r="X39" s="2"/>
+      <c r="Y39" s="2"/>
+      <c r="Z39" s="2"/>
+    </row>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A40" s="3"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="29"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+      <c r="P40" s="2"/>
+      <c r="Q40" s="2"/>
+      <c r="R40" s="2"/>
+      <c r="S40" s="2"/>
+      <c r="T40" s="2"/>
+      <c r="U40" s="2"/>
+      <c r="V40" s="2"/>
+      <c r="W40" s="2"/>
+      <c r="X40" s="2"/>
+      <c r="Y40" s="2"/>
+      <c r="Z40" s="2"/>
+    </row>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A41" s="3"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="29"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="2"/>
+      <c r="P41" s="2"/>
+      <c r="Q41" s="2"/>
+      <c r="R41" s="2"/>
+      <c r="S41" s="2"/>
+      <c r="T41" s="2"/>
+      <c r="U41" s="2"/>
+      <c r="V41" s="2"/>
+      <c r="W41" s="2"/>
+      <c r="X41" s="2"/>
+      <c r="Y41" s="2"/>
+      <c r="Z41" s="2"/>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A42" s="3"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="29"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+      <c r="O42" s="2"/>
+      <c r="P42" s="2"/>
+      <c r="Q42" s="2"/>
+      <c r="R42" s="2"/>
+      <c r="S42" s="2"/>
+      <c r="T42" s="2"/>
+      <c r="U42" s="2"/>
+      <c r="V42" s="2"/>
+      <c r="W42" s="2"/>
+      <c r="X42" s="2"/>
+      <c r="Y42" s="2"/>
+      <c r="Z42" s="2"/>
+    </row>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A43" s="3"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
+      <c r="P43" s="2"/>
+      <c r="Q43" s="2"/>
+      <c r="R43" s="2"/>
+      <c r="S43" s="2"/>
+      <c r="T43" s="2"/>
+      <c r="U43" s="2"/>
+      <c r="V43" s="2"/>
+      <c r="W43" s="2"/>
+      <c r="X43" s="2"/>
+      <c r="Y43" s="2"/>
+      <c r="Z43" s="2"/>
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A44" s="3"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="29"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="2"/>
+      <c r="P44" s="2"/>
+      <c r="Q44" s="2"/>
+      <c r="R44" s="2"/>
+      <c r="S44" s="2"/>
+      <c r="T44" s="2"/>
+      <c r="U44" s="2"/>
+      <c r="V44" s="2"/>
+      <c r="W44" s="2"/>
+      <c r="X44" s="2"/>
+      <c r="Y44" s="2"/>
+      <c r="Z44" s="2"/>
+    </row>
+    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A45" s="3"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+      <c r="O45" s="2"/>
+      <c r="P45" s="2"/>
+      <c r="Q45" s="2"/>
+      <c r="R45" s="2"/>
+      <c r="S45" s="2"/>
+      <c r="T45" s="2"/>
+      <c r="U45" s="2"/>
+      <c r="V45" s="2"/>
+      <c r="W45" s="2"/>
+      <c r="X45" s="2"/>
+      <c r="Y45" s="2"/>
+      <c r="Z45" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>